<commit_message>
logo updates on images and some pdfs
</commit_message>
<xml_diff>
--- a/static/assets/financial_analysis.xlsx
+++ b/static/assets/financial_analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattlitchliter/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattlitchliter/Documents/web/elevate-marketing-site/static/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F7A2683-E33C-804B-91A7-419E34EA4FC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C113AF6-5AD4-044D-B34D-730245A43268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21560" windowHeight="12460" xr2:uid="{5A1AF604-6E0C-4CAD-BF5D-E981E20A9721}"/>
   </bookViews>
@@ -255,7 +255,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,13 +459,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>203201</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>97059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>378969</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>93441</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -481,21 +481,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="203201" y="228600"/>
-          <a:ext cx="1572768" cy="685800"/>
+          <a:off x="203201" y="287559"/>
+          <a:ext cx="1572768" cy="567882"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -807,16 +806,16 @@
   <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A5" sqref="A5:M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="13" width="10.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -831,7 +830,7 @@
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -846,7 +845,7 @@
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="22"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -861,7 +860,7 @@
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -876,7 +875,7 @@
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
@@ -891,7 +890,7 @@
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -906,7 +905,7 @@
       <c r="L6" s="22"/>
       <c r="M6" s="22"/>
     </row>
-    <row r="7" spans="1:13" ht="21">
+    <row r="7" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>61</v>
       </c>
@@ -923,7 +922,7 @@
       <c r="L7" s="16"/>
       <c r="M7" s="16"/>
     </row>
-    <row r="9" spans="1:13" s="1" customFormat="1">
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="14" t="s">
         <v>0</v>
       </c>
@@ -961,12 +960,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>13</v>
       </c>
@@ -983,12 +982,12 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>15</v>
       </c>
@@ -1005,17 +1004,17 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>48</v>
       </c>
@@ -1032,12 +1031,12 @@
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>62</v>
       </c>
@@ -1054,12 +1053,12 @@
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>64</v>
       </c>
@@ -1076,12 +1075,12 @@
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>66</v>
       </c>
@@ -1098,12 +1097,12 @@
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>57</v>
       </c>
@@ -1120,12 +1119,12 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>50</v>
       </c>
@@ -1142,12 +1141,12 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>52</v>
       </c>
@@ -1164,7 +1163,7 @@
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:13" s="1" customFormat="1">
+    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>55</v>
       </c>
@@ -1181,20 +1180,20 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>17</v>
       </c>
@@ -1211,12 +1210,12 @@
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>63</v>
       </c>
@@ -1233,12 +1232,12 @@
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>70</v>
       </c>
@@ -1255,12 +1254,12 @@
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>18</v>
       </c>
@@ -1277,12 +1276,12 @@
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>19</v>
       </c>
@@ -1299,12 +1298,12 @@
       <c r="L42" s="7"/>
       <c r="M42" s="7"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>46</v>
       </c>
@@ -1321,12 +1320,12 @@
       <c r="L44" s="7"/>
       <c r="M44" s="7"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>22</v>
       </c>
@@ -1343,12 +1342,12 @@
       <c r="L46" s="7"/>
       <c r="M46" s="7"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>24</v>
       </c>
@@ -1365,12 +1364,12 @@
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>26</v>
       </c>
@@ -1387,12 +1386,12 @@
       <c r="L50" s="7"/>
       <c r="M50" s="7"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>28</v>
       </c>
@@ -1409,12 +1408,12 @@
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>29</v>
       </c>
@@ -1431,12 +1430,12 @@
       <c r="L54" s="7"/>
       <c r="M54" s="7"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
         <v>30</v>
       </c>
@@ -1453,12 +1452,12 @@
       <c r="L56" s="7"/>
       <c r="M56" s="7"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
         <v>32</v>
       </c>
@@ -1475,12 +1474,12 @@
       <c r="L58" s="7"/>
       <c r="M58" s="7"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
         <v>34</v>
       </c>
@@ -1497,12 +1496,12 @@
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
         <v>36</v>
       </c>
@@ -1519,12 +1518,12 @@
       <c r="L62" s="7"/>
       <c r="M62" s="7"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
         <v>38</v>
       </c>
@@ -1541,12 +1540,12 @@
       <c r="L64" s="7"/>
       <c r="M64" s="7"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>40</v>
       </c>
@@ -1563,12 +1562,12 @@
       <c r="L66" s="7"/>
       <c r="M66" s="7"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
         <v>42</v>
       </c>
@@ -1585,23 +1584,23 @@
       <c r="L68" s="7"/>
       <c r="M68" s="7"/>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
         <v>43</v>
       </c>

</xml_diff>